<commit_message>
Added test for creating multiple client instances in MailProject
</commit_message>
<xml_diff>
--- a/data/test/test_data_source.xlsx
+++ b/data/test/test_data_source.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE5C25E-6171-7B47-A4AE-E61238B8D625}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887C9EF5-D5EE-464F-877B-E4D7B147E417}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6860" yWindow="3100" windowWidth="26180" windowHeight="16460" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6860" yWindow="3100" windowWidth="26180" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="client_data" sheetId="1" r:id="rId1"/>
@@ -20,33 +20,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
   <si>
-    <t>client_id</t>
-  </si>
-  <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>address_mailing_street</t>
-  </si>
-  <si>
-    <t>address_mailing_zip</t>
-  </si>
-  <si>
-    <t>address_mailing_city</t>
-  </si>
-  <si>
-    <t>address_notify_street</t>
-  </si>
-  <si>
-    <t>address_notify_zip</t>
-  </si>
-  <si>
-    <t>address_notify_city</t>
-  </si>
-  <si>
     <t>John1</t>
   </si>
   <si>
@@ -113,21 +86,6 @@
     <t>Another Project GmbH</t>
   </si>
   <si>
-    <t>amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> subscription_am_authorized</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> mailing_as_email</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> depot_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> depot_bic</t>
-  </si>
-  <si>
     <t>1B3456789</t>
   </si>
   <si>
@@ -186,6 +144,48 @@
   </si>
   <si>
     <t>sicherheiten</t>
+  </si>
+  <si>
+    <t>db_id</t>
+  </si>
+  <si>
+    <t>name_titel_vname</t>
+  </si>
+  <si>
+    <t>name_nname</t>
+  </si>
+  <si>
+    <t>post_str</t>
+  </si>
+  <si>
+    <t>post_plz</t>
+  </si>
+  <si>
+    <t>post_ort</t>
+  </si>
+  <si>
+    <t>melde_str</t>
+  </si>
+  <si>
+    <t>melde_plz</t>
+  </si>
+  <si>
+    <t>melde_ort</t>
+  </si>
+  <si>
+    <t>zeichnungssumme</t>
+  </si>
+  <si>
+    <t>in_vv</t>
+  </si>
+  <si>
+    <t>medium_email</t>
+  </si>
+  <si>
+    <t>depot_nummer</t>
+  </si>
+  <si>
+    <t>depot_bic</t>
   </si>
 </sst>
 </file>
@@ -589,18 +589,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView zoomScale="167" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.83203125" style="3" bestFit="1" customWidth="1"/>
@@ -609,46 +612,46 @@
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>45</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
@@ -656,28 +659,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E2" s="3">
         <v>80001</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="H2" s="3">
         <v>80001</v>
       </c>
       <c r="I2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="J2">
         <v>50000</v>
@@ -692,7 +695,7 @@
         <v>123456789</v>
       </c>
       <c r="N2" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -700,28 +703,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E3" s="3">
         <v>80002</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="H3" s="3">
         <v>80002</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="J3">
         <v>1000000</v>
@@ -733,10 +736,10 @@
         <v>0</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="N3" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -744,28 +747,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
       </c>
       <c r="E4" s="3">
         <v>80003</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H4" s="3">
         <v>90003</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="J4">
         <v>10000</v>
@@ -777,10 +780,10 @@
         <v>1</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="N4" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -788,28 +791,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E5" s="3">
         <v>80004</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="H5" s="3">
         <v>90004</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="J5">
         <v>25000</v>
@@ -821,10 +824,10 @@
         <v>0</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="N5" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -838,7 +841,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView zoomScale="182" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -855,31 +858,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -887,7 +890,7 @@
         <v>141</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C2" s="4">
         <v>43646</v>
@@ -899,7 +902,7 @@
         <v>0.12</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="G2" s="6">
         <v>2000000</v>
@@ -908,7 +911,7 @@
         <v>3000000</v>
       </c>
       <c r="I2" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -922,7 +925,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -939,31 +942,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -971,7 +974,7 @@
         <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C2" s="4">
         <v>43830</v>
@@ -983,7 +986,7 @@
         <v>0.11</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="G2" s="6">
         <v>4000000</v>
@@ -992,7 +995,7 @@
         <v>5000000</v>
       </c>
       <c r="I2" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1004,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1022,31 +1025,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1054,7 +1057,7 @@
         <v>141</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C2" s="4">
         <v>43646</v>
@@ -1066,7 +1069,7 @@
         <v>0.12</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="G2" s="6">
         <v>2000000</v>
@@ -1075,7 +1078,7 @@
         <v>3000000</v>
       </c>
       <c r="I2" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1083,7 +1086,7 @@
         <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C3" s="4">
         <v>43830</v>
@@ -1095,7 +1098,7 @@
         <v>0.11</v>
       </c>
       <c r="F3" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="G3" s="6">
         <v>4000000</v>
@@ -1104,7 +1107,7 @@
         <v>5000000</v>
       </c>
       <c r="I3" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the field map and Client class to contain the title, and salutation for a client instance. Added the first merge fields for the word template 'cover_letter'
</commit_message>
<xml_diff>
--- a/data/test/test_data_source.xlsx
+++ b/data/test/test_data_source.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887C9EF5-D5EE-464F-877B-E4D7B147E417}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDC130D-71FF-1D47-A9B9-CAF722F67BB7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6860" yWindow="3100" windowWidth="26180" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4820" yWindow="5020" windowWidth="26180" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="client_data" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
   <si>
     <t>John1</t>
   </si>
@@ -149,12 +149,6 @@
     <t>db_id</t>
   </si>
   <si>
-    <t>name_titel_vname</t>
-  </si>
-  <si>
-    <t>name_nname</t>
-  </si>
-  <si>
     <t>post_str</t>
   </si>
   <si>
@@ -186,6 +180,39 @@
   </si>
   <si>
     <t>depot_bic</t>
+  </si>
+  <si>
+    <t>anrede</t>
+  </si>
+  <si>
+    <t>Herr</t>
+  </si>
+  <si>
+    <t>Frau</t>
+  </si>
+  <si>
+    <t>anrede_adressfeld</t>
+  </si>
+  <si>
+    <t>er Herr</t>
+  </si>
+  <si>
+    <t>e Frau</t>
+  </si>
+  <si>
+    <t>Herrn</t>
+  </si>
+  <si>
+    <t>titel</t>
+  </si>
+  <si>
+    <t>Dr.</t>
+  </si>
+  <si>
+    <t>vorname</t>
+  </si>
+  <si>
+    <t>nachname</t>
   </si>
 </sst>
 </file>
@@ -587,91 +614,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>55</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="3">
-        <v>80001</v>
+      <c r="E2" t="s">
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>58</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
@@ -682,40 +716,46 @@
       <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="J2">
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="3">
+        <v>80001</v>
+      </c>
+      <c r="L2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2">
         <v>50000</v>
       </c>
-      <c r="K2">
+      <c r="N2">
         <v>1</v>
       </c>
-      <c r="L2">
+      <c r="O2">
         <v>1</v>
       </c>
-      <c r="M2" s="3">
+      <c r="P2" s="3">
         <v>123456789</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3">
-        <v>80002</v>
+      <c r="E3" t="s">
+        <v>56</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -726,107 +766,131 @@
       <c r="I3" t="s">
         <v>13</v>
       </c>
-      <c r="J3">
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="3">
+        <v>80002</v>
+      </c>
+      <c r="L3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3">
         <v>1000000</v>
       </c>
-      <c r="K3">
+      <c r="N3">
         <v>1</v>
       </c>
-      <c r="L3">
+      <c r="O3">
         <v>0</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="3">
+      <c r="H4" s="3">
         <v>80003</v>
       </c>
-      <c r="F4" t="s">
+      <c r="I4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="3">
+      <c r="K4" s="3">
         <v>90003</v>
       </c>
-      <c r="I4" t="s">
+      <c r="L4" t="s">
         <v>18</v>
       </c>
-      <c r="J4">
+      <c r="M4">
         <v>10000</v>
       </c>
-      <c r="K4">
+      <c r="N4">
         <v>0</v>
       </c>
-      <c r="L4">
+      <c r="O4">
         <v>1</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N4" t="s">
+      <c r="Q4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="3">
+      <c r="H5" s="3">
         <v>80004</v>
       </c>
-      <c r="F5" t="s">
+      <c r="I5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" t="s">
+      <c r="J5" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="3">
+      <c r="K5" s="3">
         <v>90004</v>
       </c>
-      <c r="I5" t="s">
+      <c r="L5" t="s">
         <v>19</v>
       </c>
-      <c r="J5">
+      <c r="M5">
         <v>25000</v>
       </c>
-      <c r="K5">
+      <c r="N5">
         <v>0</v>
       </c>
-      <c r="L5">
+      <c r="O5">
         <v>0</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="P5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N5" t="s">
+      <c r="Q5" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added method to create word document based on 1 template.
</commit_message>
<xml_diff>
--- a/data/test/test_data_source.xlsx
+++ b/data/test/test_data_source.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDC130D-71FF-1D47-A9B9-CAF722F67BB7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC62AAB-4C12-7F4F-AAC5-857DCB749C37}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4820" yWindow="5020" windowWidth="26180" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="68">
   <si>
     <t>John1</t>
   </si>
@@ -213,6 +213,15 @@
   </si>
   <si>
     <t>nachname</t>
+  </si>
+  <si>
+    <t>betreuer</t>
+  </si>
+  <si>
+    <t>Betreuer 1</t>
+  </si>
+  <si>
+    <t>Betreuer 2</t>
   </si>
 </sst>
 </file>
@@ -614,283 +623,295 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="167" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.83203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="27.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>60</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>58</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>80001</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="3">
+      <c r="L2" s="3">
         <v>80001</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>12</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>50000</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
       </c>
       <c r="O2">
         <v>1</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="3">
         <v>123456789</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>56</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>59</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>80002</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>13</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="3">
+      <c r="L3" s="3">
         <v>80002</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>13</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>1000000</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>1</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>0</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>60</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>55</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>80003</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>14</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="3">
         <v>90003</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>18</v>
       </c>
-      <c r="M4">
-        <v>10000</v>
-      </c>
-      <c r="N4">
+      <c r="O4">
         <v>0</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>1</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
         <v>62</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>56</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>59</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>80004</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>15</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="3">
+      <c r="L5" s="3">
         <v>90004</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>19</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>25000</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
-      <c r="P5" s="3" t="s">
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>